<commit_message>
Progress towards nsti data
</commit_message>
<xml_diff>
--- a/NSTI_for_KL_variables.xlsx
+++ b/NSTI_for_KL_variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin Li\Documents\GitHub\NSTI_harborview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DB07D1-ABDD-4B68-849F-510A9AACCBFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4DD787-B631-446B-ABD0-C0E71AC11B04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{29D3DCD0-EE1F-1546-9A9E-DC47189C4449}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29D3DCD0-EE1F-1546-9A9E-DC47189C4449}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="231">
   <si>
     <t>Variable</t>
   </si>
@@ -727,6 +727,15 @@
   </si>
   <si>
     <t>Time data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admit to last operation </t>
+  </si>
+  <si>
+    <t>to when their antibiotics changed/stopped</t>
+  </si>
+  <si>
+    <t>Ground truth</t>
   </si>
 </sst>
 </file>
@@ -749,13 +758,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,6 +803,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -805,19 +834,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -833,6 +853,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159C1F83-FBF7-AB43-8393-3173DBAE852B}">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1179,18 +1224,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="8"/>
+      <c r="F1" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1275,11 +1320,11 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" t="s">
         <v>144</v>
       </c>
@@ -1288,10 +1333,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>130</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1307,17 +1352,17 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:9" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="E9" s="6" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" t="s">
         <v>148</v>
       </c>
@@ -1354,10 +1399,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1404,17 +1449,17 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1479,10 +1524,10 @@
       <c r="C21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1493,10 +1538,10 @@
       <c r="C22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="12" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1507,10 +1552,10 @@
       <c r="C23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="12" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1521,10 +1566,10 @@
       <c r="C24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="13" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1535,55 +1580,55 @@
       <c r="C25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="12" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="13" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="12" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="13" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="12" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="F30" s="1" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="F30" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="13" t="s">
         <v>194</v>
       </c>
     </row>
@@ -1602,41 +1647,41 @@
       <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="15" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>123</v>
       </c>
@@ -1647,15 +1692,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="F36" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +1714,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
@@ -1679,16 +1724,16 @@
       <c r="F38" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="39" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
       <c r="F39" s="1" t="s">
         <v>205</v>
       </c>
@@ -1696,7 +1741,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1706,11 +1751,11 @@
       <c r="F40" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
@@ -1724,7 +1769,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1734,11 +1779,11 @@
       <c r="F42" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>32</v>
       </c>
@@ -1749,7 +1794,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>34</v>
       </c>
@@ -1759,8 +1804,17 @@
       <c r="D44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
@@ -1770,8 +1824,9 @@
       <c r="D45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>36</v>
       </c>
@@ -1782,7 +1837,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>37</v>
       </c>
@@ -1793,7 +1848,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>40</v>
       </c>
@@ -2156,6 +2211,7 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>